<commit_message>
KA didn't cover everything quizzed
</commit_message>
<xml_diff>
--- a/TestSchedule.xlsx
+++ b/TestSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melton\OneDrive\Desktop\MCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AF2FF8-CB33-4DC5-94ED-02201BC74F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27ABEEC-4B5F-4EA4-B1D5-E79D1F9C2B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E159C54E-6335-4C52-82F0-BAEEAC51E9FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E159C54E-6335-4C52-82F0-BAEEAC51E9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88AA66C-3DC4-4214-89BE-05D3D6AD3882}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,7 +627,7 @@
     <col min="10" max="10" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -635,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44386</v>
       </c>
@@ -664,7 +664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44387</v>
       </c>
@@ -675,7 +675,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44388</v>
       </c>
@@ -683,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44389</v>
       </c>
@@ -705,14 +705,8 @@
       <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44390</v>
       </c>
@@ -741,7 +735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44391</v>
       </c>
@@ -769,8 +763,11 @@
       <c r="J7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44392</v>
       </c>
@@ -799,7 +796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44393</v>
       </c>
@@ -827,8 +824,11 @@
       <c r="J9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44394</v>
       </c>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44395</v>
       </c>
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44396</v>
       </c>
@@ -873,7 +873,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44397</v>
       </c>
@@ -893,7 +893,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44398</v>
       </c>
@@ -904,7 +904,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44399</v>
       </c>
@@ -915,7 +915,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44400</v>
       </c>

</xml_diff>

<commit_message>
did altius half length
</commit_message>
<xml_diff>
--- a/TestSchedule.xlsx
+++ b/TestSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melton\OneDrive\Desktop\MCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE6EC5-D30C-46B1-8FFD-B3B0884AB0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3331505E-9364-48CC-8C0E-82818417BC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20270" yWindow="1070" windowWidth="14400" windowHeight="7460" xr2:uid="{E159C54E-6335-4C52-82F0-BAEEAC51E9FD}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E159C54E-6335-4C52-82F0-BAEEAC51E9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
   <si>
     <t>TEST DAY</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>BB 64-16</t>
+  </si>
+  <si>
+    <t>Magoosh</t>
+  </si>
+  <si>
+    <t>Magoosh Review</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>BB some</t>
   </si>
 </sst>
 </file>
@@ -612,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88AA66C-3DC4-4214-89BE-05D3D6AD3882}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,28 +943,28 @@
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44401</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>69</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44402</v>
       </c>
@@ -960,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44403</v>
       </c>
@@ -968,13 +980,16 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
         <v>62</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44404</v>
       </c>
@@ -982,13 +997,19 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44405</v>
       </c>
@@ -996,13 +1017,16 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" t="s">
         <v>65</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44406</v>
       </c>
@@ -1013,7 +1037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44407</v>
       </c>
@@ -1024,7 +1048,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44408</v>
       </c>
@@ -1032,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>44409</v>
       </c>
@@ -1040,7 +1064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44410</v>
       </c>
@@ -1048,7 +1072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44411</v>
       </c>
@@ -1056,7 +1080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44412</v>
       </c>
@@ -1064,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>44413</v>
       </c>
@@ -1075,7 +1099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44414</v>
       </c>
@@ -1083,7 +1107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>44415</v>
       </c>
@@ -1091,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44416</v>
       </c>
@@ -1254,7 +1278,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D20:D21">
+  <conditionalFormatting sqref="G20:G21">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>